<commit_message>
Add dest form funksjon ferdig. Nu design.
</commit_message>
<xml_diff>
--- a/_ASSETS/climbing_grades_categorization.xlsx
+++ b/_ASSETS/climbing_grades_categorization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrerico/Desktop/climb_dest/_ASSETS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D384B6C-AB65-C24B-9B24-F49DAF5BD250}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F298C8C-EE5F-E547-91A2-FC510AD6470B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="100" windowWidth="25440" windowHeight="15360" xr2:uid="{BCDD1EB8-EB04-884F-9307-984DFD8AB761}"/>
   </bookViews>
@@ -1142,7 +1142,7 @@
   <dimension ref="E6:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>